<commit_message>
hoan thanh extract xsdp
</commit_message>
<xml_diff>
--- a/docs/cấu trúc bảng staging.xlsx
+++ b/docs/cấu trúc bảng staging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GocHocTap\eclipse\LotteryCrawler\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B4897-A4A6-476F-BDDE-84E3689C59C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE00925-9491-4495-9701-8E06C8F426B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F044F565-2541-4770-A23B-F8E484319D69}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -313,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -338,16 +338,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -356,9 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +680,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,20 +703,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -729,8 +733,8 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
@@ -872,8 +876,8 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>1</v>
+      <c r="A15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -893,9 +897,9 @@
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -916,12 +920,8 @@
       <c r="F18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -942,23 +942,19 @@
       <c r="F19" s="4">
         <v>2022</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -993,20 +989,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1142,11 +1138,11 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="7"/>
       <c r="G13" s="5">
         <v>2</v>

</xml_diff>